<commit_message>
LE0801: Ajuste de problema de fórmulas en la Solicitud gráfica
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/SolicitudGrafica_LE_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/SolicitudGrafica_LE_08_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magua_000\Documents\Planeta\Edicion\LE_08_01_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Lenguaje\fuentes\contenidos\grado08\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19203" windowHeight="8957" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="177">
   <si>
     <t>Fecha:</t>
   </si>
@@ -526,9 +526,6 @@
   </si>
   <si>
     <t>http://pixabay.com/static/uploads/photo/2012/04/18/02/19/colombia-36572_640.png</t>
-  </si>
-  <si>
-    <t>IMG01</t>
   </si>
   <si>
     <t>Pantallazo corresponde al minuto 1:40 del video. Se debe elaborar un mapa de acuerdo con la información presentada.</t>
@@ -1540,6 +1537,40 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="51" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1563,6 +1594,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1623,46 +1660,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="51" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -1846,15 +1843,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>19150</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>9575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1038225</xdr:colOff>
+          <xdr:colOff>1038873</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>239372</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1901,15 +1898,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1047750</xdr:colOff>
+          <xdr:colOff>1048448</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>9575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>866526</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>239372</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1956,15 +1953,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>19150</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>9575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>9575</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>239372</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2013,13 +2010,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>483531</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1019724</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>713328</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2066,15 +2063,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1019724</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>483531</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>828675</xdr:colOff>
+          <xdr:colOff>828226</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>713328</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2121,15 +2118,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>9575</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>483531</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>837801</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>713328</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2176,15 +2173,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>9575</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>483531</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>837801</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>713328</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2555,11 +2552,11 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:A108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.2" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.75" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="72.375" style="2" bestFit="1" customWidth="1"/>
@@ -2577,7 +2574,7 @@
     <col min="14" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2589,47 +2586,47 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="F2" s="77" t="s">
+      <c r="D2" s="97"/>
+      <c r="F2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="78"/>
+      <c r="G2" s="90"/>
       <c r="H2" s="54"/>
       <c r="I2" s="54"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="108">
+      <c r="C3" s="98">
         <v>8</v>
       </c>
-      <c r="D3" s="109"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
+      <c r="D3" s="99"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="92"/>
       <c r="H3" s="54"/>
       <c r="I3" s="54"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="87"/>
+      <c r="D4" s="101"/>
       <c r="E4" s="5"/>
       <c r="F4" s="53" t="s">
         <v>55</v>
@@ -2642,15 +2639,15 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="102" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="89"/>
+      <c r="D5" s="103"/>
       <c r="E5" s="5"/>
       <c r="F5" s="51" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2662,7 +2659,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2675,7 +2672,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1"/>
       <c r="B7" s="38" t="s">
         <v>40</v>
@@ -2693,18 +2690,18 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="95"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2713,7 +2710,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="13.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="34" t="s">
         <v>2</v>
       </c>
@@ -2748,22 +2745,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" s="110" t="s">
-        <v>153</v>
+    <row r="10" spans="1:16" s="12" customFormat="1" ht="52.8" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="str">
+        <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
+        <v>IMG01</v>
+      </c>
+      <c r="B10" s="77" t="s">
+        <v>152</v>
       </c>
       <c r="C10" s="27" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>154</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>155</v>
       </c>
       <c r="F10" s="14" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
@@ -2782,13 +2780,13 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="202.5" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="138" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="str">
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
@@ -2801,10 +2799,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F11" s="14" t="str">
         <f t="shared" ref="F11:F74" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
@@ -2822,30 +2820,30 @@
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J11" s="112" t="s">
+      <c r="J11" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="K11" s="80" t="s">
         <v>158</v>
       </c>
-      <c r="K11" s="113" t="s">
+    </row>
+    <row r="12" spans="1:16" s="12" customFormat="1" ht="31.7" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="str">
+        <f t="shared" ref="A12:A18" si="3">IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE(LEFT(A11,3),IF(MID(A11,4,2)+1&lt;10,CONCATENATE("0",MID(A11,4,2)+1))),"")</f>
+        <v>IMG03</v>
+      </c>
+      <c r="B12" s="81" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="str">
-        <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE(LEFT(A11,3),IF(MID(A11,4,2)+1&lt;10,CONCATENATE("0",MID(A11,4,2)+1))),"")</f>
-        <v>IMG03</v>
-      </c>
-      <c r="B12" s="114" t="s">
-        <v>160</v>
       </c>
       <c r="C12" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2863,28 +2861,28 @@
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12" s="115" t="s">
+      <c r="J12" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="1:16" s="12" customFormat="1" ht="31.7" x14ac:dyDescent="0.5">
+      <c r="A13" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>IMG04</v>
+      </c>
+      <c r="B13" s="84" t="s">
         <v>162</v>
-      </c>
-      <c r="K12" s="19"/>
-    </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="str">
-        <f t="shared" ref="A12:A30" si="3">IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),CONCATENATE(LEFT(A12,3),IF(MID(A12,4,2)+1&lt;10,CONCATENATE("0",MID(A12,4,2)+1))),"")</f>
-        <v>IMG04</v>
-      </c>
-      <c r="B13" s="117" t="s">
-        <v>163</v>
       </c>
       <c r="C13" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F13" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2902,28 +2900,28 @@
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J13" s="115" t="s">
-        <v>164</v>
+      <c r="J13" s="82" t="s">
+        <v>163</v>
       </c>
       <c r="K13" s="19"/>
     </row>
-    <row r="14" spans="1:16" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A14" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
       </c>
-      <c r="B14" s="117" t="s">
-        <v>165</v>
+      <c r="B14" s="84" t="s">
+        <v>164</v>
       </c>
       <c r="C14" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F14" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2941,28 +2939,28 @@
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J14" s="112" t="s">
-        <v>166</v>
+      <c r="J14" s="79" t="s">
+        <v>165</v>
       </c>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A15" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
       </c>
-      <c r="B15" s="111" t="s">
-        <v>167</v>
+      <c r="B15" s="78" t="s">
+        <v>166</v>
       </c>
       <c r="C15" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F15" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2980,28 +2978,28 @@
         <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J15" s="118" t="s">
-        <v>168</v>
+      <c r="J15" s="85" t="s">
+        <v>167</v>
       </c>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:16" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="12" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A16" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
       </c>
-      <c r="B16" s="117" t="s">
-        <v>169</v>
+      <c r="B16" s="84" t="s">
+        <v>168</v>
       </c>
       <c r="C16" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="E16" s="119" t="s">
-        <v>156</v>
+        <v>160</v>
+      </c>
+      <c r="E16" s="86" t="s">
+        <v>155</v>
       </c>
       <c r="F16" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3019,28 +3017,28 @@
         <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J16" s="120" t="s">
-        <v>170</v>
+      <c r="J16" s="87" t="s">
+        <v>169</v>
       </c>
       <c r="K16" s="35"/>
     </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="81" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="12" customFormat="1" ht="79.2" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG08</v>
       </c>
-      <c r="B17" s="116" t="s">
-        <v>171</v>
+      <c r="B17" s="83" t="s">
+        <v>170</v>
       </c>
       <c r="C17" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F17" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3058,30 +3056,30 @@
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J17" s="118" t="s">
+      <c r="J17" s="85" t="s">
+        <v>171</v>
+      </c>
+      <c r="K17" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="K17" s="118" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" s="12" customFormat="1" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A18" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG09</v>
       </c>
-      <c r="B18" s="117" t="s">
-        <v>174</v>
+      <c r="B18" s="84" t="s">
+        <v>173</v>
       </c>
       <c r="C18" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F18" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3099,32 +3097,32 @@
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J18" s="120" t="s">
+      <c r="J18" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="K18" s="21"/>
+    </row>
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="31.7" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="str">
+        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
+        <v>IMG10</v>
+      </c>
+      <c r="B19" s="88" t="s">
         <v>175</v>
-      </c>
-      <c r="K18" s="21"/>
-    </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v>IMGFALSO</v>
-      </c>
-      <c r="B19" s="121" t="s">
-        <v>176</v>
       </c>
       <c r="C19" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F19" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>LE_08_01_CO_IMGFALSO_small</v>
+        <v>LE_08_01_CO_IMG10_small</v>
       </c>
       <c r="G19" s="14" t="str">
         <f>IF(F19&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3132,20 +3130,20 @@
       </c>
       <c r="H19" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>LE_08_01_CO_IMGFALSO_zoom</v>
+        <v>LE_08_01_CO_IMG10_zoom</v>
       </c>
       <c r="I19" s="14" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J19" s="120" t="s">
-        <v>177</v>
+      <c r="J19" s="87" t="s">
+        <v>176</v>
       </c>
       <c r="K19" s="35"/>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A20:A83" si="4">IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE(LEFT(A19,3),IF(MID(A19,4,2)+1&lt;10,CONCATENATE("0",MID(A19,4,2)+1),MID(A19,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B20" s="28"/>
@@ -3174,9 +3172,9 @@
       <c r="J20" s="19"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B21" s="30"/>
@@ -3205,9 +3203,9 @@
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B22" s="31"/>
@@ -3236,9 +3234,9 @@
       <c r="J22" s="14"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B23" s="28"/>
@@ -3264,9 +3262,9 @@
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
     </row>
-    <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B24" s="27"/>
@@ -3292,9 +3290,9 @@
       <c r="J24" s="14"/>
       <c r="K24" s="15"/>
     </row>
-    <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B25" s="28"/>
@@ -3320,9 +3318,9 @@
       <c r="J25" s="14"/>
       <c r="K25" s="19"/>
     </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B26" s="28"/>
@@ -3348,9 +3346,9 @@
       <c r="J26" s="14"/>
       <c r="K26" s="19"/>
     </row>
-    <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B27" s="28"/>
@@ -3376,9 +3374,9 @@
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
     </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B28" s="27"/>
@@ -3404,9 +3402,9 @@
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
     </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B29" s="28"/>
@@ -3432,9 +3430,9 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B30" s="28"/>
@@ -3460,8 +3458,11 @@
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
+    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B31" s="28"/>
       <c r="C31" s="28"/>
       <c r="D31" s="14"/>
@@ -3485,8 +3486,11 @@
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
+    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
       <c r="D32" s="14"/>
@@ -3510,8 +3514,11 @@
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
     </row>
-    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
+    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
       <c r="D33" s="14"/>
@@ -3535,8 +3542,11 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B34" s="28"/>
       <c r="C34" s="28"/>
       <c r="D34" s="14"/>
@@ -3560,8 +3570,11 @@
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
     </row>
-    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
+    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
       <c r="D35" s="14"/>
@@ -3585,8 +3598,11 @@
       <c r="J35" s="14"/>
       <c r="K35" s="15"/>
     </row>
-    <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
+    <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B36" s="32"/>
       <c r="C36" s="32"/>
       <c r="D36" s="14"/>
@@ -3610,8 +3626,11 @@
       <c r="J36" s="14"/>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
+    <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
       <c r="D37" s="14"/>
@@ -3635,8 +3654,11 @@
       <c r="J37" s="22"/>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
+    <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B38" s="33"/>
       <c r="C38" s="33"/>
       <c r="D38" s="14"/>
@@ -3660,8 +3682,11 @@
       <c r="J38" s="23"/>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
+    <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
       <c r="D39" s="14"/>
@@ -3685,8 +3710,11 @@
       <c r="J39" s="14"/>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
+    <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B40" s="27"/>
       <c r="C40" s="27"/>
       <c r="D40" s="14"/>
@@ -3710,8 +3738,11 @@
       <c r="J40" s="14"/>
       <c r="K40" s="15"/>
     </row>
-    <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
+    <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B41" s="27"/>
       <c r="C41" s="27"/>
       <c r="D41" s="14"/>
@@ -3735,8 +3766,11 @@
       <c r="J41" s="14"/>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
+    <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B42" s="27"/>
       <c r="C42" s="27"/>
       <c r="D42" s="14"/>
@@ -3760,8 +3794,11 @@
       <c r="J42" s="14"/>
       <c r="K42" s="15"/>
     </row>
-    <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
+    <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B43" s="27"/>
       <c r="C43" s="27"/>
       <c r="D43" s="14"/>
@@ -3785,8 +3822,11 @@
       <c r="J43" s="14"/>
       <c r="K43" s="15"/>
     </row>
-    <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
+    <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
       <c r="D44" s="14"/>
@@ -3810,8 +3850,11 @@
       <c r="J44" s="14"/>
       <c r="K44" s="15"/>
     </row>
-    <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
+    <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
       <c r="D45" s="14"/>
@@ -3835,8 +3878,11 @@
       <c r="J45" s="14"/>
       <c r="K45" s="15"/>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
+    <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B46" s="27"/>
       <c r="C46" s="27"/>
       <c r="D46" s="14"/>
@@ -3860,8 +3906,11 @@
       <c r="J46" s="14"/>
       <c r="K46" s="15"/>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
+    <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B47" s="27"/>
       <c r="C47" s="27"/>
       <c r="D47" s="14"/>
@@ -3885,8 +3934,11 @@
       <c r="J47" s="14"/>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
+    <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B48" s="27"/>
       <c r="C48" s="27"/>
       <c r="D48" s="14"/>
@@ -3910,8 +3962,11 @@
       <c r="J48" s="14"/>
       <c r="K48" s="15"/>
     </row>
-    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
+    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B49" s="27"/>
       <c r="C49" s="27"/>
       <c r="D49" s="14"/>
@@ -3935,8 +3990,11 @@
       <c r="J49" s="14"/>
       <c r="K49" s="15"/>
     </row>
-    <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
+    <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B50" s="27"/>
       <c r="C50" s="27"/>
       <c r="D50" s="14"/>
@@ -3960,8 +4018,11 @@
       <c r="J50" s="14"/>
       <c r="K50" s="15"/>
     </row>
-    <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
+    <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B51" s="27"/>
       <c r="C51" s="27"/>
       <c r="D51" s="14"/>
@@ -3985,8 +4046,11 @@
       <c r="J51" s="14"/>
       <c r="K51" s="15"/>
     </row>
-    <row r="52" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
+    <row r="52" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B52" s="27"/>
       <c r="C52" s="27"/>
       <c r="D52" s="14"/>
@@ -4010,8 +4074,11 @@
       <c r="J52" s="14"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="53" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
+    <row r="53" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B53" s="27"/>
       <c r="C53" s="27"/>
       <c r="D53" s="14"/>
@@ -4035,8 +4102,11 @@
       <c r="J53" s="14"/>
       <c r="K53" s="15"/>
     </row>
-    <row r="54" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
+    <row r="54" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B54" s="27"/>
       <c r="C54" s="27"/>
       <c r="D54" s="14"/>
@@ -4060,8 +4130,11 @@
       <c r="J54" s="14"/>
       <c r="K54" s="15"/>
     </row>
-    <row r="55" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
+    <row r="55" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B55" s="27"/>
       <c r="C55" s="27"/>
       <c r="D55" s="14"/>
@@ -4085,8 +4158,11 @@
       <c r="J55" s="14"/>
       <c r="K55" s="15"/>
     </row>
-    <row r="56" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
+    <row r="56" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B56" s="27"/>
       <c r="C56" s="27"/>
       <c r="D56" s="14"/>
@@ -4110,8 +4186,11 @@
       <c r="J56" s="14"/>
       <c r="K56" s="15"/>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
+    <row r="57" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B57" s="27"/>
       <c r="C57" s="27"/>
       <c r="D57" s="14"/>
@@ -4135,8 +4214,11 @@
       <c r="J57" s="14"/>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
+    <row r="58" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B58" s="27"/>
       <c r="C58" s="27"/>
       <c r="D58" s="14"/>
@@ -4160,8 +4242,11 @@
       <c r="J58" s="14"/>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
+    <row r="59" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B59" s="27"/>
       <c r="C59" s="27"/>
       <c r="D59" s="14"/>
@@ -4185,8 +4270,11 @@
       <c r="J59" s="14"/>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
+    <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B60" s="27"/>
       <c r="C60" s="27"/>
       <c r="D60" s="14"/>
@@ -4210,8 +4298,11 @@
       <c r="J60" s="14"/>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
+    <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B61" s="27"/>
       <c r="C61" s="27"/>
       <c r="D61" s="14"/>
@@ -4235,8 +4326,11 @@
       <c r="J61" s="14"/>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
+    <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
       <c r="D62" s="14"/>
@@ -4260,8 +4354,11 @@
       <c r="J62" s="14"/>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
+    <row r="63" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
       <c r="D63" s="14"/>
@@ -4285,8 +4382,11 @@
       <c r="J63" s="14"/>
       <c r="K63" s="15"/>
     </row>
-    <row r="64" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
+    <row r="64" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
       <c r="D64" s="14"/>
@@ -4310,8 +4410,11 @@
       <c r="J64" s="14"/>
       <c r="K64" s="15"/>
     </row>
-    <row r="65" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
+    <row r="65" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
       <c r="D65" s="14"/>
@@ -4335,8 +4438,11 @@
       <c r="J65" s="14"/>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
+    <row r="66" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
       <c r="D66" s="14"/>
@@ -4360,8 +4466,11 @@
       <c r="J66" s="14"/>
       <c r="K66" s="15"/>
     </row>
-    <row r="67" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
+    <row r="67" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
       <c r="D67" s="14"/>
@@ -4385,8 +4494,11 @@
       <c r="J67" s="14"/>
       <c r="K67" s="15"/>
     </row>
-    <row r="68" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
+    <row r="68" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
       <c r="D68" s="14"/>
@@ -4410,8 +4522,11 @@
       <c r="J68" s="14"/>
       <c r="K68" s="15"/>
     </row>
-    <row r="69" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
+    <row r="69" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
       <c r="D69" s="14"/>
@@ -4435,8 +4550,11 @@
       <c r="J69" s="14"/>
       <c r="K69" s="15"/>
     </row>
-    <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
+    <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
       <c r="D70" s="14"/>
@@ -4460,8 +4578,11 @@
       <c r="J70" s="14"/>
       <c r="K70" s="15"/>
     </row>
-    <row r="71" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
+    <row r="71" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
       <c r="D71" s="14"/>
@@ -4485,8 +4606,11 @@
       <c r="J71" s="14"/>
       <c r="K71" s="15"/>
     </row>
-    <row r="72" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
+    <row r="72" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
       <c r="D72" s="14"/>
@@ -4510,8 +4634,11 @@
       <c r="J72" s="14"/>
       <c r="K72" s="15"/>
     </row>
-    <row r="73" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
+    <row r="73" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
       <c r="D73" s="14"/>
@@ -4535,8 +4662,11 @@
       <c r="J73" s="14"/>
       <c r="K73" s="15"/>
     </row>
-    <row r="74" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
+    <row r="74" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
       <c r="D74" s="14"/>
@@ -4560,14 +4690,17 @@
       <c r="J74" s="14"/>
       <c r="K74" s="15"/>
     </row>
-    <row r="75" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
+    <row r="75" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
       <c r="F75" s="14" t="str">
-        <f t="shared" ref="F75:F108" si="4">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I75="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" ref="F75:F108" si="5">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I75="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G75" s="14" t="str">
@@ -4575,7 +4708,7 @@
         <v/>
       </c>
       <c r="H75" s="14" t="str">
-        <f t="shared" ref="H75:H108" si="5">IF(I75&lt;&gt;"",IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H75:H108" si="6">IF(I75&lt;&gt;"",IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I75" s="14" t="str">
@@ -4585,14 +4718,17 @@
       <c r="J75" s="14"/>
       <c r="K75" s="15"/>
     </row>
-    <row r="76" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
+    <row r="76" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
       <c r="F76" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G76" s="14" t="str">
@@ -4600,7 +4736,7 @@
         <v/>
       </c>
       <c r="H76" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I76" s="14" t="str">
@@ -4610,14 +4746,17 @@
       <c r="J76" s="14"/>
       <c r="K76" s="15"/>
     </row>
-    <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="13"/>
+    <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
       <c r="F77" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G77" s="14" t="str">
@@ -4625,7 +4764,7 @@
         <v/>
       </c>
       <c r="H77" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I77" s="14" t="str">
@@ -4635,14 +4774,17 @@
       <c r="J77" s="14"/>
       <c r="K77" s="15"/>
     </row>
-    <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
+    <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
       <c r="F78" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G78" s="14" t="str">
@@ -4650,7 +4792,7 @@
         <v/>
       </c>
       <c r="H78" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I78" s="14" t="str">
@@ -4660,14 +4802,17 @@
       <c r="J78" s="14"/>
       <c r="K78" s="15"/>
     </row>
-    <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
+    <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
       <c r="F79" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G79" s="14" t="str">
@@ -4675,7 +4820,7 @@
         <v/>
       </c>
       <c r="H79" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I79" s="14" t="str">
@@ -4685,14 +4830,17 @@
       <c r="J79" s="14"/>
       <c r="K79" s="15"/>
     </row>
-    <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="13"/>
+    <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
       <c r="F80" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G80" s="14" t="str">
@@ -4700,7 +4848,7 @@
         <v/>
       </c>
       <c r="H80" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I80" s="14" t="str">
@@ -4710,14 +4858,17 @@
       <c r="J80" s="14"/>
       <c r="K80" s="15"/>
     </row>
-    <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
+    <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
       <c r="F81" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G81" s="14" t="str">
@@ -4725,7 +4876,7 @@
         <v/>
       </c>
       <c r="H81" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I81" s="14" t="str">
@@ -4735,14 +4886,17 @@
       <c r="J81" s="14"/>
       <c r="K81" s="15"/>
     </row>
-    <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="13"/>
+    <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
       <c r="F82" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G82" s="14" t="str">
@@ -4750,7 +4904,7 @@
         <v/>
       </c>
       <c r="H82" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I82" s="14" t="str">
@@ -4760,14 +4914,17 @@
       <c r="J82" s="14"/>
       <c r="K82" s="15"/>
     </row>
-    <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
+    <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
       <c r="F83" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G83" s="14" t="str">
@@ -4775,7 +4932,7 @@
         <v/>
       </c>
       <c r="H83" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I83" s="14" t="str">
@@ -4785,14 +4942,17 @@
       <c r="J83" s="14"/>
       <c r="K83" s="15"/>
     </row>
-    <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
+    <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="13" t="str">
+        <f t="shared" ref="A84:A108" si="7">IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),CONCATENATE(LEFT(A83,3),IF(MID(A83,4,2)+1&lt;10,CONCATENATE("0",MID(A83,4,2)+1),MID(A83,4,2)+1)),"")</f>
+        <v/>
+      </c>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
       <c r="F84" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G84" s="14" t="str">
@@ -4800,7 +4960,7 @@
         <v/>
       </c>
       <c r="H84" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I84" s="14" t="str">
@@ -4810,14 +4970,17 @@
       <c r="J84" s="14"/>
       <c r="K84" s="15"/>
     </row>
-    <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="13"/>
+    <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G85" s="14" t="str">
@@ -4825,7 +4988,7 @@
         <v/>
       </c>
       <c r="H85" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I85" s="14" t="str">
@@ -4835,14 +4998,17 @@
       <c r="J85" s="14"/>
       <c r="K85" s="15"/>
     </row>
-    <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="13"/>
+    <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
       <c r="F86" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G86" s="14" t="str">
@@ -4850,7 +5016,7 @@
         <v/>
       </c>
       <c r="H86" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I86" s="14" t="str">
@@ -4860,14 +5026,17 @@
       <c r="J86" s="14"/>
       <c r="K86" s="15"/>
     </row>
-    <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="13"/>
+    <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
       <c r="F87" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G87" s="14" t="str">
@@ -4875,7 +5044,7 @@
         <v/>
       </c>
       <c r="H87" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I87" s="14" t="str">
@@ -4885,14 +5054,17 @@
       <c r="J87" s="14"/>
       <c r="K87" s="15"/>
     </row>
-    <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="13"/>
+    <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
       <c r="F88" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G88" s="14" t="str">
@@ -4900,7 +5072,7 @@
         <v/>
       </c>
       <c r="H88" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I88" s="14" t="str">
@@ -4910,14 +5082,17 @@
       <c r="J88" s="14"/>
       <c r="K88" s="15"/>
     </row>
-    <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="13"/>
+    <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
       <c r="F89" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G89" s="14" t="str">
@@ -4925,7 +5100,7 @@
         <v/>
       </c>
       <c r="H89" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I89" s="14" t="str">
@@ -4935,14 +5110,17 @@
       <c r="J89" s="14"/>
       <c r="K89" s="15"/>
     </row>
-    <row r="90" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="13"/>
+    <row r="90" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
       <c r="F90" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G90" s="14" t="str">
@@ -4950,7 +5128,7 @@
         <v/>
       </c>
       <c r="H90" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I90" s="14" t="str">
@@ -4960,14 +5138,17 @@
       <c r="J90" s="14"/>
       <c r="K90" s="15"/>
     </row>
-    <row r="91" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="13"/>
+    <row r="91" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
       <c r="F91" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G91" s="14" t="str">
@@ -4975,7 +5156,7 @@
         <v/>
       </c>
       <c r="H91" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I91" s="14" t="str">
@@ -4985,14 +5166,17 @@
       <c r="J91" s="14"/>
       <c r="K91" s="15"/>
     </row>
-    <row r="92" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="13"/>
+    <row r="92" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
       <c r="F92" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G92" s="14" t="str">
@@ -5000,7 +5184,7 @@
         <v/>
       </c>
       <c r="H92" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I92" s="14" t="str">
@@ -5010,14 +5194,17 @@
       <c r="J92" s="14"/>
       <c r="K92" s="15"/>
     </row>
-    <row r="93" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="13"/>
+    <row r="93" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
       <c r="F93" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G93" s="14" t="str">
@@ -5025,7 +5212,7 @@
         <v/>
       </c>
       <c r="H93" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I93" s="14" t="str">
@@ -5035,14 +5222,17 @@
       <c r="J93" s="14"/>
       <c r="K93" s="15"/>
     </row>
-    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="13"/>
+    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
       <c r="F94" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G94" s="14" t="str">
@@ -5050,7 +5240,7 @@
         <v/>
       </c>
       <c r="H94" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I94" s="14" t="str">
@@ -5060,14 +5250,17 @@
       <c r="J94" s="14"/>
       <c r="K94" s="15"/>
     </row>
-    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="13"/>
+    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
       <c r="F95" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G95" s="14" t="str">
@@ -5075,7 +5268,7 @@
         <v/>
       </c>
       <c r="H95" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I95" s="14" t="str">
@@ -5085,14 +5278,17 @@
       <c r="J95" s="14"/>
       <c r="K95" s="15"/>
     </row>
-    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="13"/>
+    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
       <c r="F96" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G96" s="14" t="str">
@@ -5100,7 +5296,7 @@
         <v/>
       </c>
       <c r="H96" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I96" s="14" t="str">
@@ -5110,14 +5306,17 @@
       <c r="J96" s="14"/>
       <c r="K96" s="15"/>
     </row>
-    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="13"/>
+    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
       <c r="F97" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G97" s="14" t="str">
@@ -5125,7 +5324,7 @@
         <v/>
       </c>
       <c r="H97" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I97" s="14" t="str">
@@ -5135,14 +5334,17 @@
       <c r="J97" s="14"/>
       <c r="K97" s="15"/>
     </row>
-    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="13"/>
+    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
       <c r="F98" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G98" s="14" t="str">
@@ -5150,7 +5352,7 @@
         <v/>
       </c>
       <c r="H98" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I98" s="14" t="str">
@@ -5160,14 +5362,17 @@
       <c r="J98" s="14"/>
       <c r="K98" s="15"/>
     </row>
-    <row r="99" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="13"/>
+    <row r="99" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
       <c r="F99" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G99" s="14" t="str">
@@ -5175,7 +5380,7 @@
         <v/>
       </c>
       <c r="H99" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I99" s="14" t="str">
@@ -5185,14 +5390,17 @@
       <c r="J99" s="14"/>
       <c r="K99" s="15"/>
     </row>
-    <row r="100" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="13"/>
+    <row r="100" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
       <c r="F100" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G100" s="14" t="str">
@@ -5200,7 +5408,7 @@
         <v/>
       </c>
       <c r="H100" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I100" s="14" t="str">
@@ -5210,14 +5418,17 @@
       <c r="J100" s="14"/>
       <c r="K100" s="15"/>
     </row>
-    <row r="101" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="13"/>
+    <row r="101" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
       <c r="F101" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G101" s="14" t="str">
@@ -5225,7 +5436,7 @@
         <v/>
       </c>
       <c r="H101" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I101" s="14" t="str">
@@ -5235,14 +5446,17 @@
       <c r="J101" s="14"/>
       <c r="K101" s="15"/>
     </row>
-    <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="13"/>
+    <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B102" s="13"/>
       <c r="C102" s="13"/>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
       <c r="F102" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G102" s="14" t="str">
@@ -5250,7 +5464,7 @@
         <v/>
       </c>
       <c r="H102" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I102" s="14" t="str">
@@ -5260,14 +5474,17 @@
       <c r="J102" s="14"/>
       <c r="K102" s="15"/>
     </row>
-    <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="13"/>
+    <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B103" s="13"/>
       <c r="C103" s="13"/>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
       <c r="F103" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G103" s="14" t="str">
@@ -5275,7 +5492,7 @@
         <v/>
       </c>
       <c r="H103" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I103" s="14" t="str">
@@ -5285,14 +5502,17 @@
       <c r="J103" s="14"/>
       <c r="K103" s="15"/>
     </row>
-    <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="13"/>
+    <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B104" s="13"/>
       <c r="C104" s="13"/>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
       <c r="F104" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G104" s="14" t="str">
@@ -5300,7 +5520,7 @@
         <v/>
       </c>
       <c r="H104" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I104" s="14" t="str">
@@ -5310,14 +5530,17 @@
       <c r="J104" s="14"/>
       <c r="K104" s="15"/>
     </row>
-    <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="13"/>
+    <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B105" s="13"/>
       <c r="C105" s="13"/>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
       <c r="F105" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G105" s="14" t="str">
@@ -5325,7 +5548,7 @@
         <v/>
       </c>
       <c r="H105" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I105" s="14" t="str">
@@ -5335,14 +5558,17 @@
       <c r="J105" s="14"/>
       <c r="K105" s="15"/>
     </row>
-    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="13"/>
+    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B106" s="13"/>
       <c r="C106" s="13"/>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
       <c r="F106" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G106" s="14" t="str">
@@ -5350,7 +5576,7 @@
         <v/>
       </c>
       <c r="H106" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I106" s="14" t="str">
@@ -5360,14 +5586,17 @@
       <c r="J106" s="14"/>
       <c r="K106" s="15"/>
     </row>
-    <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="13"/>
+    <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B107" s="13"/>
       <c r="C107" s="13"/>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
       <c r="F107" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G107" s="14" t="str">
@@ -5375,7 +5604,7 @@
         <v/>
       </c>
       <c r="H107" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I107" s="14" t="str">
@@ -5385,14 +5614,17 @@
       <c r="J107" s="14"/>
       <c r="K107" s="15"/>
     </row>
-    <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="13"/>
+    <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="B108" s="13"/>
       <c r="C108" s="13"/>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
       <c r="F108" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G108" s="14" t="str">
@@ -5400,7 +5632,7 @@
         <v/>
       </c>
       <c r="H108" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I108" s="14" t="str">
@@ -5486,7 +5718,7 @@
       <selection activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.85" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="72.25" style="36" customWidth="1"/>
     <col min="2" max="2" width="11" style="36"/>
@@ -5497,38 +5729,38 @@
     <col min="12" max="16384" width="11" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="92" t="s">
+    <row r="1" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="94"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="108"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="44" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="45"/>
-      <c r="C2" s="95" t="s">
+      <c r="C2" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="111"/>
       <c r="F2" s="46"/>
     </row>
-    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A3" s="47" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="45"/>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="102"/>
-      <c r="E3" s="103"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117"/>
       <c r="F3" s="46"/>
       <c r="H3" s="36" t="s">
         <v>18</v>
@@ -5543,7 +5775,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A4" s="44" t="s">
         <v>44</v>
       </c>
@@ -5571,7 +5803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="79.55" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="47" t="s">
         <v>45</v>
       </c>
@@ -5579,11 +5811,11 @@
       <c r="C5" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="104" t="str">
+      <c r="D5" s="118" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_08_01_CO</v>
       </c>
-      <c r="E5" s="105"/>
+      <c r="E5" s="119"/>
       <c r="F5" s="46"/>
       <c r="H5" s="36" t="s">
         <v>22</v>
@@ -5598,7 +5830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="44" t="s">
         <v>10</v>
       </c>
@@ -5620,7 +5852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="47" t="s">
         <v>11</v>
       </c>
@@ -5628,12 +5860,12 @@
       <c r="C7" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="90" t="str">
+      <c r="D7" s="104" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_08_01_CO.xls</v>
       </c>
-      <c r="E7" s="90"/>
-      <c r="F7" s="91"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="105"/>
       <c r="H7" s="36" t="s">
         <v>24</v>
       </c>
@@ -5647,7 +5879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="47.5" x14ac:dyDescent="0.5">
       <c r="A8" s="47" t="s">
         <v>53</v>
       </c>
@@ -5666,7 +5898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="47.5" x14ac:dyDescent="0.5">
       <c r="A9" s="47" t="s">
         <v>12</v>
       </c>
@@ -5685,7 +5917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="48" t="s">
         <v>36</v>
       </c>
@@ -5704,7 +5936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="I11" s="36" t="s">
         <v>32</v>
       </c>
@@ -5715,7 +5947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="I12" s="36" t="s">
         <v>37</v>
       </c>
@@ -5726,15 +5958,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="92" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A13" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="94"/>
+      <c r="B13" s="107"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="108"/>
       <c r="I13" s="36" t="s">
         <v>33</v>
       </c>
@@ -5745,7 +5977,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="47"/>
       <c r="B14" s="45"/>
       <c r="C14" s="45"/>
@@ -5762,17 +5994,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="44" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="45"/>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="111"/>
       <c r="J15" s="36">
         <v>12</v>
       </c>
@@ -5780,7 +6012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="67.2" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="47" t="s">
         <v>47</v>
       </c>
@@ -5804,7 +6036,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="32.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="44" t="s">
         <v>44</v>
       </c>
@@ -5812,12 +6044,12 @@
       <c r="C17" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="98" t="str">
+      <c r="D17" s="112" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_08_01_REC10</v>
       </c>
-      <c r="E17" s="99"/>
-      <c r="F17" s="100"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="114"/>
       <c r="J17" s="36">
         <v>14</v>
       </c>
@@ -5825,7 +6057,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="79.55" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="47" t="s">
         <v>48</v>
       </c>
@@ -5833,12 +6065,12 @@
       <c r="C18" s="76" t="s">
         <v>144</v>
       </c>
-      <c r="D18" s="90" t="str">
+      <c r="D18" s="104" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_08_01_REC10.xls</v>
       </c>
-      <c r="E18" s="90"/>
-      <c r="F18" s="91"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="105"/>
       <c r="J18" s="36">
         <v>15</v>
       </c>
@@ -5846,7 +6078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19" s="44" t="s">
         <v>10</v>
       </c>
@@ -5865,7 +6097,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="48" t="s">
         <v>51</v>
       </c>
@@ -5887,7 +6119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="H21" s="36" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -5904,122 +6136,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K22" s="36">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K23" s="36">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K24" s="36">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K25" s="36">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K26" s="36">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K27" s="36">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K28" s="36">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K29" s="36">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K30" s="36">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K31" s="36">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K32" s="36">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K33" s="36">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K34" s="36">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K35" s="36">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K36" s="36">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K37" s="36">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K38" s="36">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K39" s="36">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K40" s="36">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K41" s="36">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K42" s="36">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K43" s="36">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K44" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K45" s="36" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -6053,13 +6285,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>483531</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1019724</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>713328</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6073,15 +6305,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1019724</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>483531</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>828675</xdr:colOff>
+                    <xdr:colOff>828226</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>713328</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6095,15 +6327,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>9575</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>483531</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>838200</xdr:colOff>
+                    <xdr:colOff>837801</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>713328</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6117,15 +6349,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>9575</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>483531</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>838200</xdr:colOff>
+                    <xdr:colOff>837801</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>713328</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6139,15 +6371,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>19150</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>9575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1038225</xdr:colOff>
+                    <xdr:colOff>1038873</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>239372</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6161,15 +6393,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1047750</xdr:colOff>
+                    <xdr:colOff>1048448</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>9575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>866775</xdr:colOff>
+                    <xdr:colOff>866526</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>239372</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6183,15 +6415,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>19150</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>9575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>9575</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>239372</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6213,7 +6445,7 @@
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.85" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="21" style="36" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="36" customWidth="1"/>
@@ -6228,42 +6460,42 @@
     <col min="12" max="16384" width="10.875" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A1" s="120" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="107" t="s">
+      <c r="H1" s="121" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="106"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A2" s="120"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
       <c r="H2" s="55" t="s">
         <v>65</v>
       </c>
@@ -6274,7 +6506,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A3" s="56" t="s">
         <v>69</v>
       </c>
@@ -6298,7 +6530,7 @@
       <c r="I3" s="56"/>
       <c r="J3" s="56"/>
     </row>
-    <row r="4" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A4" s="58" t="s">
         <v>57</v>
       </c>
@@ -6326,7 +6558,7 @@
       </c>
       <c r="J4" s="58"/>
     </row>
-    <row r="5" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A5" s="59" t="s">
         <v>80</v>
       </c>
@@ -6354,7 +6586,7 @@
       </c>
       <c r="J5" s="60"/>
     </row>
-    <row r="6" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A6" s="58" t="s">
         <v>58</v>
       </c>
@@ -6386,7 +6618,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="57" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="57" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A7" s="58" t="s">
         <v>84</v>
       </c>
@@ -6414,7 +6646,7 @@
       </c>
       <c r="J7" s="58"/>
     </row>
-    <row r="8" spans="1:11" s="57" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="58" t="s">
         <v>86</v>
       </c>
@@ -6442,7 +6674,7 @@
       </c>
       <c r="J8" s="58"/>
     </row>
-    <row r="9" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="58" t="s">
         <v>88</v>
       </c>
@@ -6470,7 +6702,7 @@
       </c>
       <c r="J9" s="58"/>
     </row>
-    <row r="10" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="58" t="s">
         <v>90</v>
       </c>
@@ -6494,7 +6726,7 @@
       <c r="I10" s="58"/>
       <c r="J10" s="58"/>
     </row>
-    <row r="11" spans="1:11" s="57" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="57" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A11" s="58" t="s">
         <v>93</v>
       </c>
@@ -6522,7 +6754,7 @@
       </c>
       <c r="J11" s="58"/>
     </row>
-    <row r="12" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="58" t="s">
         <v>95</v>
       </c>
@@ -6550,7 +6782,7 @@
       </c>
       <c r="J12" s="58"/>
     </row>
-    <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A13" s="61" t="s">
         <v>97</v>
       </c>
@@ -6577,7 +6809,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="61" t="s">
         <v>101</v>
       </c>
@@ -6601,7 +6833,7 @@
       </c>
       <c r="J14" s="61"/>
     </row>
-    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A15" s="61" t="s">
         <v>103</v>
       </c>
@@ -6628,7 +6860,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="95" x14ac:dyDescent="0.5">
       <c r="A16" s="63" t="s">
         <v>107</v>
       </c>
@@ -6657,7 +6889,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A17" s="58" t="s">
         <v>112</v>
       </c>
@@ -6686,12 +6918,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" s="67" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" s="68" t="s">
         <v>119</v>
       </c>
@@ -6704,7 +6936,7 @@
       <c r="D21" s="69"/>
       <c r="E21" s="69"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22" s="71" t="s">
         <v>122</v>
       </c>
@@ -6717,7 +6949,7 @@
       <c r="D22" s="72"/>
       <c r="E22" s="72"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" s="71" t="s">
         <v>125</v>
       </c>
@@ -6730,7 +6962,7 @@
       <c r="D23" s="72"/>
       <c r="E23" s="72"/>
     </row>
-    <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A24" s="71" t="s">
         <v>128</v>
       </c>
@@ -6743,7 +6975,7 @@
       <c r="D24" s="72"/>
       <c r="E24" s="72"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25" s="71" t="s">
         <v>131</v>
       </c>
@@ -6756,7 +6988,7 @@
       <c r="D25" s="72"/>
       <c r="E25" s="72"/>
     </row>
-    <row r="26" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A26" s="71" t="s">
         <v>134</v>
       </c>

</xml_diff>